<commit_message>
Actualizacion documetacion y automatizacion
</commit_message>
<xml_diff>
--- a/Plan de Pruebas EC1 (3) (2).xlsx
+++ b/Plan de Pruebas EC1 (3) (2).xlsx
@@ -8,10 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Plan de Pruebas" sheetId="1" r:id="rId1"/>
-    <sheet name="Estrategia" sheetId="5" r:id="rId2"/>
-    <sheet name="Supuestos" sheetId="3" r:id="rId3"/>
-    <sheet name="Estimacion - Desglose" sheetId="2" r:id="rId4"/>
-    <sheet name="Factor de Ajuste" sheetId="4" r:id="rId5"/>
+    <sheet name="Estimacion - Desglose" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -233,33 +230,8 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Jhon Sebastián Rodríguez Rodríguez</author>
-  </authors>
-  <commentList>
-    <comment ref="A5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Causales de desfase:
-https://wiki.choucairtesting.com/wiki/index.php/Clasificaci%C3%B3n_Desfases</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="126">
   <si>
     <r>
       <rPr>
@@ -417,121 +389,6 @@
   </si>
   <si>
     <t>Revisa este ejemplo</t>
-  </si>
-  <si>
-    <t>AUTOEVALUACIÓN</t>
-  </si>
-  <si>
-    <t>Planteamiento de Estrategias  de Pruebas</t>
-  </si>
-  <si>
-    <t>Aspecto a evaluar</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>¿Consideró solicitar contexto del proyecto para otros aspectos como: Arquitectura, análisis técnico, sistemas externos?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Consideró otros aspectos diferentes al funcional para verificar en la solución de software? </t>
-  </si>
-  <si>
-    <t>¿Consideró cómo hacer más eficientes las pruebas ?</t>
-  </si>
-  <si>
-    <t>¿Qué técnicas está sugiriendo?(Exploratory Testing, automatización, Técnicas de selección entre otras.)</t>
-  </si>
-  <si>
-    <t>¿Se identifican productos de prueba que ayuden a mitigar riesgos?</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">¿La estrategia es coherente con los riesgos identificados? </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri Light"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve">Lo más crítico es primero.  Apuntar la estrategia a lo más crítico </t>
-    </r>
-  </si>
-  <si>
-    <t>¿La estrategia de proyecto apunta a cumplir con las restricciones del cliente?</t>
-  </si>
-  <si>
-    <t>¿El orden de ejecución que se plantea es el adecuado?</t>
-  </si>
-  <si>
-    <t>¿La estimación y el cronograma están basados en la estrategia planteada?</t>
-  </si>
-  <si>
-    <t>¿El alcance identificado está basado en los riesgos?</t>
-  </si>
-  <si>
-    <t>¿Se está considerando la sincronización entre equipos de prueba?</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Supuestos:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Para el inicio de la prueba se cuentan con los siguientes supuestos: 
--Toda la documentación necesaria para elaborar la versión del plan de pruebas ha sido suministrada al analista de pruebas  el día DD/MM/AAAA. Si se entrega documentación posterior a esta fecha en las que se especifique modificaciones a las funcionalidades existentes o adición de nuevas funcionalidades se generarán cambios en el plan de pruebas, cronograma y el diseño de los casos de prueba, que afectarán directamente los tiempos de la prueba.
--La ejecución de las pruebas se realizará en un ambiente similar al ambiente de producción.
-Los usuarios de bases de datos, sistemas operativos, aplicativos y recursos necesarios para realizar la prueba serán proporcionados por Soluciones innovadoras S.A.S. y tendrán todos los permisos y privilegios necesarios para operar adecuadamente la aplicación.
--Los analistas contarán con las herramientas de consulta, ejecución y/o editores necesarios para ejecutar los casos de prueba.
--Se espera contar con un ambiente de pruebas estable.
--Desarrollo debe realizar sus pruebas unitarias y entregarlas como suministro para iniciar las pruebas.
--Se cuenta con los desarrollos en su versión final para la ejecución de la prueba.
-El equipo de desarrollo tendrá la disposición de solucionar y despejar lo más pronto posible las dudas e inconvenientes que se presenten relacionadas con el ambiente de pruebas y temas del negocio.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nota:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Choucair sólo es responsable de la funcionalidad incluida en la documentación del proyecto generada a la fecha de entrega del mismo. Choucair incluirá dichas funcionalidades en el plan de pruebas, el cual debe ser verificado y aprobado por el cliente.
-</t>
-    </r>
   </si>
   <si>
     <t>Etapa / Actividades</t>
@@ -660,231 +517,6 @@
     <t>Total dias</t>
   </si>
   <si>
-    <t>Causales de Desfase</t>
-  </si>
-  <si>
-    <t>Valor porcentual</t>
-  </si>
-  <si>
-    <t>Factor de ajuste se define por medio de:</t>
-  </si>
-  <si>
-    <r>
-      <t>Mala calidad de artefacto recibido-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Desarrollo</t>
-    </r>
-  </si>
-  <si>
-    <t>Porcentaje fijo establecido por cliente y choucair que puede ser del 35%</t>
-  </si>
-  <si>
-    <r>
-      <t>Alistamiento de ambientes-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ambientes QA</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Datos historicos en base a proyectos anteriores teniendo en cuenta causales de desfase y porcentaje de factor de ajuste </t>
-  </si>
-  <si>
-    <r>
-      <t>Pendiente de Instalación Por Infraestructura-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Infraestructura</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Cambio de alcance-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Gestion de la Demanda</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Riesgos de proyecto identificados y valorados </t>
-  </si>
-  <si>
-    <r>
-      <t>Administración y control de versiones o releases de software-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Versiones</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Desconocimiento negocio-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Fabrica QA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Incumplimiento en la entrega de artefactos(Pend Entrega del desarrollo)-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Desarrollo</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Gestión issues(Bloqueado por defecto)-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Desarrollo</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Inestabilidad del ambiente de pruebas durante la ejecución - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Infraestructura</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Actividades de SW o HW no planeadas-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Infraestructura QA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Ejecución en ambientes compartidos-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Release Management</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Novedades equipo de trabajo, Actividades del proyecto no planeadas -</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>QA</t>
-    </r>
-  </si>
-  <si>
-    <t>Eventos externos</t>
-  </si>
-  <si>
-    <t>Total Factor de ajuste para el tipo de prueba</t>
-  </si>
-  <si>
-    <t>&lt;=35%</t>
-  </si>
-  <si>
-    <t>&lt;=25%</t>
-  </si>
-  <si>
-    <t>CH</t>
-  </si>
-  <si>
-    <t>Clientes</t>
-  </si>
-  <si>
     <t>Corporativo</t>
   </si>
   <si>
@@ -982,9 +614,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>OTRA</t>
   </si>
   <si>
     <t>Lectura de documentación</t>
@@ -1123,7 +752,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1345,50 +974,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri Light"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri Light"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri Light"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1396,7 +981,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1412,12 +997,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1451,20 +1030,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="29">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1605,54 +1172,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1784,30 +1308,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1816,7 +1316,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1833,13 +1333,13 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1854,43 +1354,43 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1902,16 +1402,16 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1920,119 +1420,136 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="29" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="29" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="8" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="10" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2042,14 +1559,92 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2063,12 +1658,18 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2081,203 +1682,26 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2318,7 +1742,7 @@
         <xdr:cNvPr id="7" name="1 Grupo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2337,7 +1761,7 @@
           <xdr:cNvPr id="8" name="2 Triángulo isósceles">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2381,7 +1805,7 @@
           <xdr:cNvPr id="9" name="3 CuadroTexto">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2433,7 +1857,7 @@
           <xdr:cNvPr id="10" name="4 CuadroTexto">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2484,7 +1908,7 @@
           <xdr:cNvPr id="11" name="5 CuadroTexto">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2553,7 +1977,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2616,7 +2040,7 @@
         <xdr:cNvPr id="13" name="Flecha: a la derecha 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C8F414B-1B05-424D-AEBD-0397129D474E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2C8F414B-1B05-424D-AEBD-0397129D474E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2671,75 +2095,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2085975</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3124200</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="1 Rectángulo redondeado">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2085975" y="5715000"/>
-          <a:ext cx="1038225" cy="381000"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1600" b="1">
-              <a:latin typeface="Tw Cen MT" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Volver</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>65943</xdr:colOff>
       <xdr:row>43</xdr:row>
@@ -2756,7 +2111,7 @@
         <xdr:cNvPr id="2" name="Flecha: a la derecha 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F11EFA6-F96F-4D3C-A0D7-86F7F846B3A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F11EFA6-F96F-4D3C-A0D7-86F7F846B3A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3091,7 +2446,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3101,8 +2456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A88" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65:I73"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52:I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3120,152 +2475,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
     </row>
     <row r="2" spans="2:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="119"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="85"/>
     </row>
     <row r="3" spans="2:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
     </row>
     <row r="4" spans="2:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
     </row>
     <row r="5" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="122" t="s">
+      <c r="B5" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="123"/>
-      <c r="H5" s="123"/>
-      <c r="I5" s="124"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="88"/>
     </row>
     <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="120" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="120"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="120"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="121"/>
+      <c r="C6" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="60"/>
     </row>
     <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="120" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="120"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="120"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="120"/>
-      <c r="I7" s="121"/>
+      <c r="C7" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="60"/>
     </row>
     <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="145" t="s">
+      <c r="B8" s="78" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="120"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="120"/>
-      <c r="G8" s="120"/>
-      <c r="H8" s="120"/>
-      <c r="I8" s="121"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="60"/>
     </row>
     <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="145"/>
+      <c r="B9" s="78"/>
       <c r="C9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="120"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="121"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="60"/>
     </row>
     <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="145"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="120"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="120"/>
-      <c r="I10" s="121"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="60"/>
     </row>
     <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="120" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
-      <c r="H11" s="120"/>
-      <c r="I11" s="121"/>
+      <c r="C11" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="60"/>
     </row>
     <row r="12" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="130" t="s">
-        <v>159</v>
-      </c>
-      <c r="D12" s="131"/>
-      <c r="E12" s="131"/>
-      <c r="F12" s="131"/>
-      <c r="G12" s="131"/>
-      <c r="H12" s="131"/>
-      <c r="I12" s="132"/>
+      <c r="C12" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="63"/>
     </row>
     <row r="13" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.25">
@@ -3281,76 +2636,76 @@
       <c r="I14" s="19"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="133" t="s">
-        <v>158</v>
-      </c>
-      <c r="C15" s="134"/>
-      <c r="D15" s="134"/>
-      <c r="E15" s="134"/>
-      <c r="F15" s="134"/>
-      <c r="G15" s="134"/>
-      <c r="H15" s="134"/>
-      <c r="I15" s="135"/>
+      <c r="B15" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="66"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="133"/>
-      <c r="C16" s="134"/>
-      <c r="D16" s="134"/>
-      <c r="E16" s="134"/>
-      <c r="F16" s="134"/>
-      <c r="G16" s="134"/>
-      <c r="H16" s="134"/>
-      <c r="I16" s="135"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="66"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="133"/>
-      <c r="C17" s="134"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="134"/>
-      <c r="F17" s="134"/>
-      <c r="G17" s="134"/>
-      <c r="H17" s="134"/>
-      <c r="I17" s="135"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="66"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="133"/>
-      <c r="C18" s="134"/>
-      <c r="D18" s="134"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="134"/>
-      <c r="G18" s="134"/>
-      <c r="H18" s="134"/>
-      <c r="I18" s="135"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="66"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="133"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="134"/>
-      <c r="E19" s="134"/>
-      <c r="F19" s="134"/>
-      <c r="G19" s="134"/>
-      <c r="H19" s="134"/>
-      <c r="I19" s="135"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="66"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="133"/>
-      <c r="C20" s="134"/>
-      <c r="D20" s="134"/>
-      <c r="E20" s="134"/>
-      <c r="F20" s="134"/>
-      <c r="G20" s="134"/>
-      <c r="H20" s="134"/>
-      <c r="I20" s="135"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="66"/>
     </row>
     <row r="21" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="136"/>
-      <c r="C21" s="137"/>
-      <c r="D21" s="137"/>
-      <c r="E21" s="137"/>
-      <c r="F21" s="137"/>
-      <c r="G21" s="137"/>
-      <c r="H21" s="137"/>
-      <c r="I21" s="138"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="69"/>
     </row>
     <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="20"/>
@@ -3363,54 +2718,54 @@
       <c r="I22" s="20"/>
     </row>
     <row r="23" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="139" t="s">
+      <c r="B23" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="140"/>
-      <c r="D23" s="140"/>
-      <c r="E23" s="140"/>
-      <c r="F23" s="140"/>
-      <c r="G23" s="140"/>
-      <c r="H23" s="140"/>
-      <c r="I23" s="141"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="72"/>
     </row>
     <row r="24" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="127" t="s">
+      <c r="B24" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="128"/>
-      <c r="D24" s="128"/>
-      <c r="E24" s="128"/>
-      <c r="F24" s="129" t="s">
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="129"/>
-      <c r="H24" s="129"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
       <c r="I24" s="25" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="142" t="s">
+      <c r="B25" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="143"/>
-      <c r="D25" s="143"/>
-      <c r="E25" s="143"/>
-      <c r="F25" s="143"/>
-      <c r="G25" s="143"/>
-      <c r="H25" s="143"/>
-      <c r="I25" s="144"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="75"/>
     </row>
     <row r="26" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B26" s="115" t="s">
+      <c r="B26" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="116"/>
-      <c r="D26" s="116" t="s">
+      <c r="C26" s="77"/>
+      <c r="D26" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="116"/>
+      <c r="E26" s="77"/>
       <c r="F26" s="23" t="s">
         <v>18</v>
       </c>
@@ -3425,14 +2780,14 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="74" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75" t="s">
-        <v>110</v>
-      </c>
-      <c r="E27" s="75"/>
+      <c r="B27" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="80"/>
+      <c r="D27" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="80"/>
       <c r="F27" s="28">
         <v>3</v>
       </c>
@@ -3443,19 +2798,19 @@
         <f t="shared" ref="H27:H32" si="0">F27*G27</f>
         <v>6</v>
       </c>
-      <c r="I27" s="72" t="s">
-        <v>116</v>
+      <c r="I27" s="52" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="74" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="75"/>
-      <c r="D28" s="76" t="s">
-        <v>111</v>
-      </c>
-      <c r="E28" s="76"/>
+      <c r="B28" s="79" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="80"/>
+      <c r="D28" s="81" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="81"/>
       <c r="F28" s="28">
         <v>3</v>
       </c>
@@ -3466,19 +2821,19 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I28" s="72" t="s">
-        <v>117</v>
+      <c r="I28" s="52" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="74" t="s">
-        <v>125</v>
-      </c>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75" t="s">
-        <v>112</v>
-      </c>
-      <c r="E29" s="75"/>
+      <c r="B29" s="79" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="80"/>
+      <c r="D29" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="80"/>
       <c r="F29" s="28">
         <v>2</v>
       </c>
@@ -3489,19 +2844,19 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I29" s="72" t="s">
-        <v>115</v>
+      <c r="I29" s="52" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="74" t="s">
-        <v>109</v>
-      </c>
-      <c r="C30" s="76"/>
-      <c r="D30" s="75" t="s">
-        <v>113</v>
-      </c>
-      <c r="E30" s="75"/>
+      <c r="B30" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="81"/>
+      <c r="D30" s="80" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="80"/>
       <c r="F30" s="28">
         <v>3</v>
       </c>
@@ -3512,19 +2867,19 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I30" s="72" t="s">
-        <v>114</v>
+      <c r="I30" s="52" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="74" t="s">
-        <v>126</v>
-      </c>
-      <c r="C31" s="75"/>
-      <c r="D31" s="76" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" s="76"/>
+      <c r="B31" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="80"/>
+      <c r="D31" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" s="81"/>
       <c r="F31" s="28">
         <v>3</v>
       </c>
@@ -3535,19 +2890,19 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="I31" s="72" t="s">
-        <v>130</v>
+      <c r="I31" s="52" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="2:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B32" s="110" t="s">
-        <v>127</v>
-      </c>
-      <c r="C32" s="76"/>
-      <c r="D32" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="E32" s="75"/>
+      <c r="B32" s="89" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="81"/>
+      <c r="D32" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="80"/>
       <c r="F32" s="28">
         <v>3</v>
       </c>
@@ -3558,8 +2913,8 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="I32" s="72" t="s">
-        <v>129</v>
+      <c r="I32" s="52" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3567,22 +2922,22 @@
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="62"/>
-      <c r="H33" s="62"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="51"/>
       <c r="I33" s="22" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="34" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="115" t="s">
+      <c r="B34" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="116"/>
-      <c r="D34" s="116" t="s">
+      <c r="C34" s="77"/>
+      <c r="D34" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="116"/>
+      <c r="E34" s="77"/>
       <c r="F34" s="23" t="s">
         <v>18</v>
       </c>
@@ -3595,22 +2950,22 @@
       <c r="I34" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="J34" s="77" t="s">
+      <c r="J34" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="K34" s="78"/>
-      <c r="L34" s="78"/>
-      <c r="M34" s="79"/>
+      <c r="K34" s="116"/>
+      <c r="L34" s="116"/>
+      <c r="M34" s="117"/>
     </row>
     <row r="35" spans="2:13" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="110" t="s">
-        <v>118</v>
-      </c>
-      <c r="C35" s="76"/>
-      <c r="D35" s="76" t="s">
-        <v>119</v>
-      </c>
-      <c r="E35" s="76"/>
+      <c r="B35" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="81"/>
+      <c r="D35" s="81" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="81"/>
       <c r="F35" s="28">
         <v>2</v>
       </c>
@@ -3622,22 +2977,22 @@
         <v>2</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="J35" s="84"/>
-      <c r="K35" s="85"/>
-      <c r="L35" s="85"/>
-      <c r="M35" s="86"/>
+        <v>81</v>
+      </c>
+      <c r="J35" s="118"/>
+      <c r="K35" s="82"/>
+      <c r="L35" s="82"/>
+      <c r="M35" s="119"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="110" t="s">
-        <v>120</v>
-      </c>
-      <c r="C36" s="76"/>
-      <c r="D36" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" s="76"/>
+      <c r="B36" s="89" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="81"/>
+      <c r="D36" s="81" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" s="81"/>
       <c r="F36" s="28">
         <v>3</v>
       </c>
@@ -3649,18 +3004,18 @@
         <v>9</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="2:13" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="110" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76" t="s">
-        <v>123</v>
-      </c>
-      <c r="E37" s="76"/>
+      <c r="B37" s="89" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="81"/>
+      <c r="D37" s="81" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="81"/>
       <c r="F37" s="28">
         <v>3</v>
       </c>
@@ -3672,22 +3027,22 @@
         <v>3</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="J37" s="84"/>
-      <c r="K37" s="85"/>
-      <c r="L37" s="85"/>
-      <c r="M37" s="86"/>
+        <v>83</v>
+      </c>
+      <c r="J37" s="118"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="82"/>
+      <c r="M37" s="119"/>
     </row>
     <row r="38" spans="2:13" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="110" t="s">
-        <v>132</v>
-      </c>
-      <c r="C38" s="76"/>
-      <c r="D38" s="76" t="s">
-        <v>133</v>
-      </c>
-      <c r="E38" s="76"/>
+      <c r="B38" s="89" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="81"/>
+      <c r="D38" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" s="81"/>
       <c r="F38" s="28">
         <v>3</v>
       </c>
@@ -3699,18 +3054,18 @@
         <v>3</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="J38" s="84"/>
-      <c r="K38" s="85"/>
-      <c r="L38" s="85"/>
-      <c r="M38" s="86"/>
+        <v>93</v>
+      </c>
+      <c r="J38" s="118"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="82"/>
+      <c r="M38" s="119"/>
     </row>
     <row r="39" spans="2:13" s="3" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="111"/>
-      <c r="C39" s="112"/>
-      <c r="D39" s="112"/>
-      <c r="E39" s="112"/>
+      <c r="B39" s="95"/>
+      <c r="C39" s="96"/>
+      <c r="D39" s="96"/>
+      <c r="E39" s="96"/>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
       <c r="H39" s="11">
@@ -3718,10 +3073,10 @@
         <v>0</v>
       </c>
       <c r="I39" s="5"/>
-      <c r="J39" s="87"/>
-      <c r="K39" s="88"/>
-      <c r="L39" s="88"/>
-      <c r="M39" s="89"/>
+      <c r="J39" s="120"/>
+      <c r="K39" s="121"/>
+      <c r="L39" s="121"/>
+      <c r="M39" s="122"/>
     </row>
     <row r="40" spans="2:13" s="3" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="2:13" ht="15" x14ac:dyDescent="0.25">
@@ -3738,11 +3093,11 @@
     </row>
     <row r="42" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
-      <c r="C42" s="113" t="s">
+      <c r="C42" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="113"/>
-      <c r="E42" s="113"/>
+      <c r="D42" s="90"/>
+      <c r="E42" s="90"/>
       <c r="F42" s="26" t="s">
         <v>26</v>
       </c>
@@ -3755,81 +3110,81 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="94" t="s">
+      <c r="B43" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="114" t="s">
-        <v>160</v>
-      </c>
-      <c r="D43" s="95"/>
-      <c r="E43" s="95"/>
-      <c r="F43" s="93" t="s">
-        <v>137</v>
-      </c>
-      <c r="G43" s="93"/>
-      <c r="H43" s="93"/>
+      <c r="C43" s="92" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="93"/>
+      <c r="E43" s="93"/>
+      <c r="F43" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="G43" s="94"/>
+      <c r="H43" s="94"/>
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="94"/>
-      <c r="C44" s="95"/>
-      <c r="D44" s="95"/>
-      <c r="E44" s="95"/>
-      <c r="F44" s="93"/>
-      <c r="G44" s="93"/>
-      <c r="H44" s="93"/>
+      <c r="B44" s="91"/>
+      <c r="C44" s="93"/>
+      <c r="D44" s="93"/>
+      <c r="E44" s="93"/>
+      <c r="F44" s="94"/>
+      <c r="G44" s="94"/>
+      <c r="H44" s="94"/>
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="94" t="s">
+      <c r="B45" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="108" t="s">
-        <v>161</v>
-      </c>
-      <c r="D45" s="109"/>
-      <c r="E45" s="109"/>
-      <c r="F45" s="93"/>
-      <c r="G45" s="93" t="s">
-        <v>137</v>
-      </c>
-      <c r="H45" s="93"/>
+      <c r="C45" s="97" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" s="98"/>
+      <c r="E45" s="98"/>
+      <c r="F45" s="94"/>
+      <c r="G45" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="H45" s="94"/>
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="2:13" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="94"/>
-      <c r="C46" s="109"/>
-      <c r="D46" s="109"/>
-      <c r="E46" s="109"/>
-      <c r="F46" s="93"/>
-      <c r="G46" s="93"/>
-      <c r="H46" s="93"/>
+      <c r="B46" s="91"/>
+      <c r="C46" s="98"/>
+      <c r="D46" s="98"/>
+      <c r="E46" s="98"/>
+      <c r="F46" s="94"/>
+      <c r="G46" s="94"/>
+      <c r="H46" s="94"/>
       <c r="I46" s="10"/>
     </row>
     <row r="47" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="94" t="s">
+      <c r="B47" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="95" t="s">
-        <v>162</v>
-      </c>
-      <c r="D47" s="95"/>
-      <c r="E47" s="95"/>
-      <c r="F47" s="93" t="s">
-        <v>137</v>
-      </c>
-      <c r="G47" s="93"/>
-      <c r="H47" s="93"/>
+      <c r="C47" s="93" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" s="93"/>
+      <c r="E47" s="93"/>
+      <c r="F47" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="G47" s="94"/>
+      <c r="H47" s="94"/>
       <c r="I47" s="10"/>
     </row>
     <row r="48" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="94"/>
-      <c r="C48" s="95"/>
-      <c r="D48" s="95"/>
-      <c r="E48" s="95"/>
-      <c r="F48" s="93"/>
-      <c r="G48" s="93"/>
-      <c r="H48" s="93"/>
+      <c r="B48" s="91"/>
+      <c r="C48" s="93"/>
+      <c r="D48" s="93"/>
+      <c r="E48" s="93"/>
+      <c r="F48" s="94"/>
+      <c r="G48" s="94"/>
+      <c r="H48" s="94"/>
       <c r="I48" s="10"/>
     </row>
     <row r="49" spans="2:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3844,126 +3199,126 @@
     </row>
     <row r="50" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="2:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="90" t="s">
+      <c r="B51" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="91"/>
-      <c r="D51" s="91"/>
-      <c r="E51" s="91"/>
-      <c r="F51" s="91"/>
-      <c r="G51" s="91"/>
-      <c r="H51" s="91"/>
-      <c r="I51" s="92"/>
+      <c r="C51" s="124"/>
+      <c r="D51" s="124"/>
+      <c r="E51" s="124"/>
+      <c r="F51" s="124"/>
+      <c r="G51" s="124"/>
+      <c r="H51" s="124"/>
+      <c r="I51" s="125"/>
     </row>
     <row r="52" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="74"/>
-      <c r="C52" s="75"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="75"/>
-      <c r="G52" s="75"/>
-      <c r="H52" s="75"/>
-      <c r="I52" s="80"/>
+      <c r="B52" s="79"/>
+      <c r="C52" s="80"/>
+      <c r="D52" s="80"/>
+      <c r="E52" s="80"/>
+      <c r="F52" s="80"/>
+      <c r="G52" s="80"/>
+      <c r="H52" s="80"/>
+      <c r="I52" s="111"/>
     </row>
     <row r="53" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="74"/>
-      <c r="C53" s="75"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="75"/>
-      <c r="F53" s="75"/>
-      <c r="G53" s="75"/>
-      <c r="H53" s="75"/>
-      <c r="I53" s="80"/>
+      <c r="B53" s="79"/>
+      <c r="C53" s="80"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="80"/>
+      <c r="F53" s="80"/>
+      <c r="G53" s="80"/>
+      <c r="H53" s="80"/>
+      <c r="I53" s="111"/>
     </row>
     <row r="54" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="74"/>
-      <c r="C54" s="75"/>
-      <c r="D54" s="75"/>
-      <c r="E54" s="75"/>
-      <c r="F54" s="75"/>
-      <c r="G54" s="75"/>
-      <c r="H54" s="75"/>
-      <c r="I54" s="80"/>
+      <c r="B54" s="79"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="80"/>
+      <c r="E54" s="80"/>
+      <c r="F54" s="80"/>
+      <c r="G54" s="80"/>
+      <c r="H54" s="80"/>
+      <c r="I54" s="111"/>
     </row>
     <row r="55" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="74"/>
-      <c r="C55" s="75"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="75"/>
-      <c r="F55" s="75"/>
-      <c r="G55" s="75"/>
-      <c r="H55" s="75"/>
-      <c r="I55" s="80"/>
+      <c r="B55" s="79"/>
+      <c r="C55" s="80"/>
+      <c r="D55" s="80"/>
+      <c r="E55" s="80"/>
+      <c r="F55" s="80"/>
+      <c r="G55" s="80"/>
+      <c r="H55" s="80"/>
+      <c r="I55" s="111"/>
     </row>
     <row r="56" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="74"/>
-      <c r="C56" s="75"/>
-      <c r="D56" s="75"/>
-      <c r="E56" s="75"/>
-      <c r="F56" s="75"/>
-      <c r="G56" s="75"/>
-      <c r="H56" s="75"/>
-      <c r="I56" s="80"/>
+      <c r="B56" s="79"/>
+      <c r="C56" s="80"/>
+      <c r="D56" s="80"/>
+      <c r="E56" s="80"/>
+      <c r="F56" s="80"/>
+      <c r="G56" s="80"/>
+      <c r="H56" s="80"/>
+      <c r="I56" s="111"/>
     </row>
     <row r="57" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="74"/>
-      <c r="C57" s="75"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="75"/>
-      <c r="F57" s="75"/>
-      <c r="G57" s="75"/>
-      <c r="H57" s="75"/>
-      <c r="I57" s="80"/>
+      <c r="B57" s="79"/>
+      <c r="C57" s="80"/>
+      <c r="D57" s="80"/>
+      <c r="E57" s="80"/>
+      <c r="F57" s="80"/>
+      <c r="G57" s="80"/>
+      <c r="H57" s="80"/>
+      <c r="I57" s="111"/>
     </row>
     <row r="58" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="74"/>
-      <c r="C58" s="75"/>
-      <c r="D58" s="75"/>
-      <c r="E58" s="75"/>
-      <c r="F58" s="75"/>
-      <c r="G58" s="75"/>
-      <c r="H58" s="75"/>
-      <c r="I58" s="80"/>
+      <c r="B58" s="79"/>
+      <c r="C58" s="80"/>
+      <c r="D58" s="80"/>
+      <c r="E58" s="80"/>
+      <c r="F58" s="80"/>
+      <c r="G58" s="80"/>
+      <c r="H58" s="80"/>
+      <c r="I58" s="111"/>
     </row>
     <row r="59" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="74"/>
-      <c r="C59" s="75"/>
-      <c r="D59" s="75"/>
-      <c r="E59" s="75"/>
-      <c r="F59" s="75"/>
-      <c r="G59" s="75"/>
-      <c r="H59" s="75"/>
-      <c r="I59" s="80"/>
+      <c r="B59" s="79"/>
+      <c r="C59" s="80"/>
+      <c r="D59" s="80"/>
+      <c r="E59" s="80"/>
+      <c r="F59" s="80"/>
+      <c r="G59" s="80"/>
+      <c r="H59" s="80"/>
+      <c r="I59" s="111"/>
     </row>
     <row r="60" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="74"/>
-      <c r="C60" s="75"/>
-      <c r="D60" s="75"/>
-      <c r="E60" s="75"/>
-      <c r="F60" s="75"/>
-      <c r="G60" s="75"/>
-      <c r="H60" s="75"/>
-      <c r="I60" s="80"/>
+      <c r="B60" s="79"/>
+      <c r="C60" s="80"/>
+      <c r="D60" s="80"/>
+      <c r="E60" s="80"/>
+      <c r="F60" s="80"/>
+      <c r="G60" s="80"/>
+      <c r="H60" s="80"/>
+      <c r="I60" s="111"/>
     </row>
     <row r="61" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="81"/>
-      <c r="C61" s="82"/>
-      <c r="D61" s="82"/>
-      <c r="E61" s="82"/>
-      <c r="F61" s="82"/>
-      <c r="G61" s="82"/>
-      <c r="H61" s="82"/>
-      <c r="I61" s="83"/>
+      <c r="B61" s="112"/>
+      <c r="C61" s="113"/>
+      <c r="D61" s="113"/>
+      <c r="E61" s="113"/>
+      <c r="F61" s="113"/>
+      <c r="G61" s="113"/>
+      <c r="H61" s="113"/>
+      <c r="I61" s="114"/>
     </row>
     <row r="62" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="85"/>
-      <c r="C62" s="85"/>
-      <c r="D62" s="85"/>
-      <c r="E62" s="85"/>
-      <c r="F62" s="85"/>
-      <c r="G62" s="85"/>
-      <c r="H62" s="85"/>
-      <c r="I62" s="85"/>
+      <c r="B62" s="82"/>
+      <c r="C62" s="82"/>
+      <c r="D62" s="82"/>
+      <c r="E62" s="82"/>
+      <c r="F62" s="82"/>
+      <c r="G62" s="82"/>
+      <c r="H62" s="82"/>
+      <c r="I62" s="82"/>
     </row>
     <row r="63" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B63" s="17" t="s">
@@ -3978,200 +3333,200 @@
       <c r="I63" s="19"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="96" t="s">
+      <c r="B64" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="C64" s="97"/>
-      <c r="D64" s="97"/>
-      <c r="E64" s="97"/>
-      <c r="F64" s="97"/>
-      <c r="G64" s="97"/>
-      <c r="H64" s="97"/>
-      <c r="I64" s="98"/>
+      <c r="C64" s="100"/>
+      <c r="D64" s="100"/>
+      <c r="E64" s="100"/>
+      <c r="F64" s="100"/>
+      <c r="G64" s="100"/>
+      <c r="H64" s="100"/>
+      <c r="I64" s="101"/>
     </row>
     <row r="65" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="74"/>
-      <c r="C65" s="75"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="75"/>
-      <c r="H65" s="75"/>
-      <c r="I65" s="80"/>
+      <c r="B65" s="79"/>
+      <c r="C65" s="80"/>
+      <c r="D65" s="80"/>
+      <c r="E65" s="80"/>
+      <c r="F65" s="80"/>
+      <c r="G65" s="80"/>
+      <c r="H65" s="80"/>
+      <c r="I65" s="111"/>
     </row>
     <row r="66" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="74"/>
-      <c r="C66" s="75"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="75"/>
-      <c r="H66" s="75"/>
-      <c r="I66" s="80"/>
+      <c r="B66" s="79"/>
+      <c r="C66" s="80"/>
+      <c r="D66" s="80"/>
+      <c r="E66" s="80"/>
+      <c r="F66" s="80"/>
+      <c r="G66" s="80"/>
+      <c r="H66" s="80"/>
+      <c r="I66" s="111"/>
     </row>
     <row r="67" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="74"/>
-      <c r="C67" s="75"/>
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
-      <c r="G67" s="75"/>
-      <c r="H67" s="75"/>
-      <c r="I67" s="80"/>
+      <c r="B67" s="79"/>
+      <c r="C67" s="80"/>
+      <c r="D67" s="80"/>
+      <c r="E67" s="80"/>
+      <c r="F67" s="80"/>
+      <c r="G67" s="80"/>
+      <c r="H67" s="80"/>
+      <c r="I67" s="111"/>
     </row>
     <row r="68" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="74"/>
-      <c r="C68" s="75"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="75"/>
-      <c r="F68" s="75"/>
-      <c r="G68" s="75"/>
-      <c r="H68" s="75"/>
-      <c r="I68" s="80"/>
+      <c r="B68" s="79"/>
+      <c r="C68" s="80"/>
+      <c r="D68" s="80"/>
+      <c r="E68" s="80"/>
+      <c r="F68" s="80"/>
+      <c r="G68" s="80"/>
+      <c r="H68" s="80"/>
+      <c r="I68" s="111"/>
     </row>
     <row r="69" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="74"/>
-      <c r="C69" s="75"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="75"/>
-      <c r="F69" s="75"/>
-      <c r="G69" s="75"/>
-      <c r="H69" s="75"/>
-      <c r="I69" s="80"/>
+      <c r="B69" s="79"/>
+      <c r="C69" s="80"/>
+      <c r="D69" s="80"/>
+      <c r="E69" s="80"/>
+      <c r="F69" s="80"/>
+      <c r="G69" s="80"/>
+      <c r="H69" s="80"/>
+      <c r="I69" s="111"/>
     </row>
     <row r="70" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="74"/>
-      <c r="C70" s="75"/>
-      <c r="D70" s="75"/>
-      <c r="E70" s="75"/>
-      <c r="F70" s="75"/>
-      <c r="G70" s="75"/>
-      <c r="H70" s="75"/>
-      <c r="I70" s="80"/>
+      <c r="B70" s="79"/>
+      <c r="C70" s="80"/>
+      <c r="D70" s="80"/>
+      <c r="E70" s="80"/>
+      <c r="F70" s="80"/>
+      <c r="G70" s="80"/>
+      <c r="H70" s="80"/>
+      <c r="I70" s="111"/>
     </row>
     <row r="71" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="74"/>
-      <c r="C71" s="75"/>
-      <c r="D71" s="75"/>
-      <c r="E71" s="75"/>
-      <c r="F71" s="75"/>
-      <c r="G71" s="75"/>
-      <c r="H71" s="75"/>
-      <c r="I71" s="80"/>
+      <c r="B71" s="79"/>
+      <c r="C71" s="80"/>
+      <c r="D71" s="80"/>
+      <c r="E71" s="80"/>
+      <c r="F71" s="80"/>
+      <c r="G71" s="80"/>
+      <c r="H71" s="80"/>
+      <c r="I71" s="111"/>
     </row>
     <row r="72" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="74"/>
-      <c r="C72" s="75"/>
-      <c r="D72" s="75"/>
-      <c r="E72" s="75"/>
-      <c r="F72" s="75"/>
-      <c r="G72" s="75"/>
-      <c r="H72" s="75"/>
-      <c r="I72" s="80"/>
+      <c r="B72" s="79"/>
+      <c r="C72" s="80"/>
+      <c r="D72" s="80"/>
+      <c r="E72" s="80"/>
+      <c r="F72" s="80"/>
+      <c r="G72" s="80"/>
+      <c r="H72" s="80"/>
+      <c r="I72" s="111"/>
     </row>
     <row r="73" spans="2:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="74"/>
-      <c r="C73" s="75"/>
-      <c r="D73" s="75"/>
-      <c r="E73" s="75"/>
-      <c r="F73" s="75"/>
-      <c r="G73" s="75"/>
-      <c r="H73" s="75"/>
-      <c r="I73" s="80"/>
+      <c r="B73" s="79"/>
+      <c r="C73" s="80"/>
+      <c r="D73" s="80"/>
+      <c r="E73" s="80"/>
+      <c r="F73" s="80"/>
+      <c r="G73" s="80"/>
+      <c r="H73" s="80"/>
+      <c r="I73" s="111"/>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B74" s="96" t="s">
+      <c r="B74" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="C74" s="97"/>
-      <c r="D74" s="97"/>
-      <c r="E74" s="97"/>
-      <c r="F74" s="97"/>
-      <c r="G74" s="97"/>
-      <c r="H74" s="97"/>
-      <c r="I74" s="98"/>
+      <c r="C74" s="100"/>
+      <c r="D74" s="100"/>
+      <c r="E74" s="100"/>
+      <c r="F74" s="100"/>
+      <c r="G74" s="100"/>
+      <c r="H74" s="100"/>
+      <c r="I74" s="101"/>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" s="74" t="s">
-        <v>163</v>
-      </c>
-      <c r="C75" s="75"/>
-      <c r="D75" s="75"/>
-      <c r="E75" s="75"/>
-      <c r="F75" s="75"/>
-      <c r="G75" s="75"/>
-      <c r="H75" s="75"/>
-      <c r="I75" s="80"/>
+      <c r="B75" s="79" t="s">
+        <v>121</v>
+      </c>
+      <c r="C75" s="80"/>
+      <c r="D75" s="80"/>
+      <c r="E75" s="80"/>
+      <c r="F75" s="80"/>
+      <c r="G75" s="80"/>
+      <c r="H75" s="80"/>
+      <c r="I75" s="111"/>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B76" s="74"/>
-      <c r="C76" s="75"/>
-      <c r="D76" s="75"/>
-      <c r="E76" s="75"/>
-      <c r="F76" s="75"/>
-      <c r="G76" s="75"/>
-      <c r="H76" s="75"/>
-      <c r="I76" s="80"/>
+      <c r="B76" s="79"/>
+      <c r="C76" s="80"/>
+      <c r="D76" s="80"/>
+      <c r="E76" s="80"/>
+      <c r="F76" s="80"/>
+      <c r="G76" s="80"/>
+      <c r="H76" s="80"/>
+      <c r="I76" s="111"/>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" s="74"/>
-      <c r="C77" s="75"/>
-      <c r="D77" s="75"/>
-      <c r="E77" s="75"/>
-      <c r="F77" s="75"/>
-      <c r="G77" s="75"/>
-      <c r="H77" s="75"/>
-      <c r="I77" s="80"/>
+      <c r="B77" s="79"/>
+      <c r="C77" s="80"/>
+      <c r="D77" s="80"/>
+      <c r="E77" s="80"/>
+      <c r="F77" s="80"/>
+      <c r="G77" s="80"/>
+      <c r="H77" s="80"/>
+      <c r="I77" s="111"/>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" s="74"/>
-      <c r="C78" s="75"/>
-      <c r="D78" s="75"/>
-      <c r="E78" s="75"/>
-      <c r="F78" s="75"/>
-      <c r="G78" s="75"/>
-      <c r="H78" s="75"/>
-      <c r="I78" s="80"/>
+      <c r="B78" s="79"/>
+      <c r="C78" s="80"/>
+      <c r="D78" s="80"/>
+      <c r="E78" s="80"/>
+      <c r="F78" s="80"/>
+      <c r="G78" s="80"/>
+      <c r="H78" s="80"/>
+      <c r="I78" s="111"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B79" s="74"/>
-      <c r="C79" s="75"/>
-      <c r="D79" s="75"/>
-      <c r="E79" s="75"/>
-      <c r="F79" s="75"/>
-      <c r="G79" s="75"/>
-      <c r="H79" s="75"/>
-      <c r="I79" s="80"/>
+      <c r="B79" s="79"/>
+      <c r="C79" s="80"/>
+      <c r="D79" s="80"/>
+      <c r="E79" s="80"/>
+      <c r="F79" s="80"/>
+      <c r="G79" s="80"/>
+      <c r="H79" s="80"/>
+      <c r="I79" s="111"/>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B80" s="74"/>
-      <c r="C80" s="75"/>
-      <c r="D80" s="75"/>
-      <c r="E80" s="75"/>
-      <c r="F80" s="75"/>
-      <c r="G80" s="75"/>
-      <c r="H80" s="75"/>
-      <c r="I80" s="80"/>
+      <c r="B80" s="79"/>
+      <c r="C80" s="80"/>
+      <c r="D80" s="80"/>
+      <c r="E80" s="80"/>
+      <c r="F80" s="80"/>
+      <c r="G80" s="80"/>
+      <c r="H80" s="80"/>
+      <c r="I80" s="111"/>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B81" s="74"/>
-      <c r="C81" s="75"/>
-      <c r="D81" s="75"/>
-      <c r="E81" s="75"/>
-      <c r="F81" s="75"/>
-      <c r="G81" s="75"/>
-      <c r="H81" s="75"/>
-      <c r="I81" s="80"/>
+      <c r="B81" s="79"/>
+      <c r="C81" s="80"/>
+      <c r="D81" s="80"/>
+      <c r="E81" s="80"/>
+      <c r="F81" s="80"/>
+      <c r="G81" s="80"/>
+      <c r="H81" s="80"/>
+      <c r="I81" s="111"/>
     </row>
     <row r="82" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="81"/>
-      <c r="C82" s="82"/>
-      <c r="D82" s="82"/>
-      <c r="E82" s="82"/>
-      <c r="F82" s="82"/>
-      <c r="G82" s="82"/>
-      <c r="H82" s="82"/>
-      <c r="I82" s="83"/>
+      <c r="B82" s="112"/>
+      <c r="C82" s="113"/>
+      <c r="D82" s="113"/>
+      <c r="E82" s="113"/>
+      <c r="F82" s="113"/>
+      <c r="G82" s="113"/>
+      <c r="H82" s="113"/>
+      <c r="I82" s="114"/>
     </row>
     <row r="84" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="B84" s="6" t="s">
@@ -4198,113 +3553,172 @@
       <c r="I85" s="7"/>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B86" s="99" t="s">
-        <v>164</v>
-      </c>
-      <c r="C86" s="100"/>
-      <c r="D86" s="100"/>
-      <c r="E86" s="100"/>
-      <c r="F86" s="100"/>
-      <c r="G86" s="100"/>
-      <c r="H86" s="100"/>
-      <c r="I86" s="101"/>
+      <c r="B86" s="102" t="s">
+        <v>122</v>
+      </c>
+      <c r="C86" s="103"/>
+      <c r="D86" s="103"/>
+      <c r="E86" s="103"/>
+      <c r="F86" s="103"/>
+      <c r="G86" s="103"/>
+      <c r="H86" s="103"/>
+      <c r="I86" s="104"/>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B87" s="102"/>
-      <c r="C87" s="103"/>
-      <c r="D87" s="103"/>
-      <c r="E87" s="103"/>
-      <c r="F87" s="103"/>
-      <c r="G87" s="103"/>
-      <c r="H87" s="103"/>
-      <c r="I87" s="104"/>
+      <c r="B87" s="105"/>
+      <c r="C87" s="106"/>
+      <c r="D87" s="106"/>
+      <c r="E87" s="106"/>
+      <c r="F87" s="106"/>
+      <c r="G87" s="106"/>
+      <c r="H87" s="106"/>
+      <c r="I87" s="107"/>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B88" s="102"/>
-      <c r="C88" s="103"/>
-      <c r="D88" s="103"/>
-      <c r="E88" s="103"/>
-      <c r="F88" s="103"/>
-      <c r="G88" s="103"/>
-      <c r="H88" s="103"/>
-      <c r="I88" s="104"/>
+      <c r="B88" s="105"/>
+      <c r="C88" s="106"/>
+      <c r="D88" s="106"/>
+      <c r="E88" s="106"/>
+      <c r="F88" s="106"/>
+      <c r="G88" s="106"/>
+      <c r="H88" s="106"/>
+      <c r="I88" s="107"/>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B89" s="102"/>
-      <c r="C89" s="103"/>
-      <c r="D89" s="103"/>
-      <c r="E89" s="103"/>
-      <c r="F89" s="103"/>
-      <c r="G89" s="103"/>
-      <c r="H89" s="103"/>
-      <c r="I89" s="104"/>
+      <c r="B89" s="105"/>
+      <c r="C89" s="106"/>
+      <c r="D89" s="106"/>
+      <c r="E89" s="106"/>
+      <c r="F89" s="106"/>
+      <c r="G89" s="106"/>
+      <c r="H89" s="106"/>
+      <c r="I89" s="107"/>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B90" s="102"/>
-      <c r="C90" s="103"/>
-      <c r="D90" s="103"/>
-      <c r="E90" s="103"/>
-      <c r="F90" s="103"/>
-      <c r="G90" s="103"/>
-      <c r="H90" s="103"/>
-      <c r="I90" s="104"/>
+      <c r="B90" s="105"/>
+      <c r="C90" s="106"/>
+      <c r="D90" s="106"/>
+      <c r="E90" s="106"/>
+      <c r="F90" s="106"/>
+      <c r="G90" s="106"/>
+      <c r="H90" s="106"/>
+      <c r="I90" s="107"/>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B91" s="102"/>
-      <c r="C91" s="103"/>
-      <c r="D91" s="103"/>
-      <c r="E91" s="103"/>
-      <c r="F91" s="103"/>
-      <c r="G91" s="103"/>
-      <c r="H91" s="103"/>
-      <c r="I91" s="104"/>
+      <c r="B91" s="105"/>
+      <c r="C91" s="106"/>
+      <c r="D91" s="106"/>
+      <c r="E91" s="106"/>
+      <c r="F91" s="106"/>
+      <c r="G91" s="106"/>
+      <c r="H91" s="106"/>
+      <c r="I91" s="107"/>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B92" s="102"/>
-      <c r="C92" s="103"/>
-      <c r="D92" s="103"/>
-      <c r="E92" s="103"/>
-      <c r="F92" s="103"/>
-      <c r="G92" s="103"/>
-      <c r="H92" s="103"/>
-      <c r="I92" s="104"/>
+      <c r="B92" s="105"/>
+      <c r="C92" s="106"/>
+      <c r="D92" s="106"/>
+      <c r="E92" s="106"/>
+      <c r="F92" s="106"/>
+      <c r="G92" s="106"/>
+      <c r="H92" s="106"/>
+      <c r="I92" s="107"/>
     </row>
     <row r="93" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B93" s="102"/>
-      <c r="C93" s="103"/>
-      <c r="D93" s="103"/>
-      <c r="E93" s="103"/>
-      <c r="F93" s="103"/>
-      <c r="G93" s="103"/>
-      <c r="H93" s="103"/>
-      <c r="I93" s="104"/>
-      <c r="J93" s="125" t="s">
+      <c r="B93" s="105"/>
+      <c r="C93" s="106"/>
+      <c r="D93" s="106"/>
+      <c r="E93" s="106"/>
+      <c r="F93" s="106"/>
+      <c r="G93" s="106"/>
+      <c r="H93" s="106"/>
+      <c r="I93" s="107"/>
+      <c r="J93" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="K93" s="126"/>
+      <c r="K93" s="55"/>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B94" s="102"/>
-      <c r="C94" s="103"/>
-      <c r="D94" s="103"/>
-      <c r="E94" s="103"/>
-      <c r="F94" s="103"/>
-      <c r="G94" s="103"/>
-      <c r="H94" s="103"/>
-      <c r="I94" s="104"/>
+      <c r="B94" s="105"/>
+      <c r="C94" s="106"/>
+      <c r="D94" s="106"/>
+      <c r="E94" s="106"/>
+      <c r="F94" s="106"/>
+      <c r="G94" s="106"/>
+      <c r="H94" s="106"/>
+      <c r="I94" s="107"/>
     </row>
     <row r="95" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="105"/>
-      <c r="C95" s="106"/>
-      <c r="D95" s="106"/>
-      <c r="E95" s="106"/>
-      <c r="F95" s="106"/>
-      <c r="G95" s="106"/>
-      <c r="H95" s="106"/>
-      <c r="I95" s="107"/>
+      <c r="B95" s="108"/>
+      <c r="C95" s="109"/>
+      <c r="D95" s="109"/>
+      <c r="E95" s="109"/>
+      <c r="F95" s="109"/>
+      <c r="G95" s="109"/>
+      <c r="H95" s="109"/>
+      <c r="I95" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="75">
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="B52:I61"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="B51:I51"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:E48"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="B74:I74"/>
+    <mergeCell ref="B86:I95"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="E62:I62"/>
+    <mergeCell ref="B64:I64"/>
+    <mergeCell ref="B65:I73"/>
+    <mergeCell ref="B75:I82"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="J93:K93"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="F24:H24"/>
@@ -4321,65 +3735,6 @@
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="B74:I74"/>
-    <mergeCell ref="B86:I95"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="E62:I62"/>
-    <mergeCell ref="B64:I64"/>
-    <mergeCell ref="B65:I73"/>
-    <mergeCell ref="B75:I82"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="B52:I61"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="B51:I51"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:E48"/>
   </mergeCells>
   <conditionalFormatting sqref="H27:H32 H36">
     <cfRule type="colorScale" priority="2">
@@ -4413,188 +3768,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="52.42578125" style="64" customWidth="1"/>
-    <col min="2" max="3" width="4.5703125" style="63" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="63"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="146" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="146"/>
-      <c r="C2" s="146"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="66" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="70" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" s="70"/>
-      <c r="G5" s="69"/>
-    </row>
-    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="71" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="70"/>
-      <c r="G6" s="69"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="63" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="67" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="67" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="70" t="s">
-        <v>137</v>
-      </c>
-      <c r="C10" s="70"/>
-    </row>
-    <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="70" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" s="70"/>
-    </row>
-    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="68" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="68" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="70" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="70"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="68" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="70" t="s">
-        <v>137</v>
-      </c>
-      <c r="C14" s="70"/>
-    </row>
-    <row r="15" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="68" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="70" t="s">
-        <v>137</v>
-      </c>
-      <c r="C15" s="70"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:D2"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="83.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="4:4" ht="405.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="61" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView showGridLines="0" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4611,36 +3789,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="148" t="s">
-        <v>56</v>
+      <c r="A1" s="129" t="s">
+        <v>39</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="149" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="149" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="149" t="s">
-        <v>61</v>
+        <v>41</v>
+      </c>
+      <c r="D1" s="126" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="126" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="126" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="148"/>
+      <c r="A2" s="129"/>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -4653,7 +3831,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="D4" s="35">
         <v>4</v>
@@ -4664,7 +3842,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="D5" s="35">
         <v>7</v>
@@ -4685,7 +3863,7 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B8" s="40"/>
       <c r="C8" s="40"/>
@@ -4695,14 +3873,14 @@
         <f>SUM(D9:D14)</f>
         <v>16</v>
       </c>
-      <c r="G8" s="150" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" s="150"/>
+      <c r="G8" s="127" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="127"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>141</v>
+        <v>99</v>
       </c>
       <c r="D9" s="35">
         <v>4</v>
@@ -4710,12 +3888,12 @@
       <c r="E9" s="35">
         <v>3</v>
       </c>
-      <c r="G9" s="150"/>
-      <c r="H9" s="150"/>
+      <c r="G9" s="127"/>
+      <c r="H9" s="127"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>142</v>
+        <v>100</v>
       </c>
       <c r="D10" s="35">
         <v>4</v>
@@ -4723,12 +3901,12 @@
       <c r="E10" s="35">
         <v>3</v>
       </c>
-      <c r="G10" s="150"/>
-      <c r="H10" s="150"/>
+      <c r="G10" s="127"/>
+      <c r="H10" s="127"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>143</v>
+        <v>101</v>
       </c>
       <c r="D11" s="35">
         <v>2</v>
@@ -4736,12 +3914,12 @@
       <c r="E11" s="35">
         <v>3</v>
       </c>
-      <c r="G11" s="150"/>
-      <c r="H11" s="150"/>
+      <c r="G11" s="127"/>
+      <c r="H11" s="127"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="D12" s="35">
         <v>2</v>
@@ -4749,12 +3927,12 @@
       <c r="E12" s="35">
         <v>3</v>
       </c>
-      <c r="G12" s="150"/>
-      <c r="H12" s="150"/>
+      <c r="G12" s="127"/>
+      <c r="H12" s="127"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="D13" s="35">
         <v>2</v>
@@ -4762,12 +3940,12 @@
       <c r="E13" s="35">
         <v>3</v>
       </c>
-      <c r="G13" s="150"/>
-      <c r="H13" s="150"/>
+      <c r="G13" s="127"/>
+      <c r="H13" s="127"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="D14" s="35">
         <v>2</v>
@@ -4775,12 +3953,12 @@
       <c r="E14" s="35">
         <v>3</v>
       </c>
-      <c r="G14" s="150"/>
-      <c r="H14" s="150"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="127"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" s="40"/>
@@ -4788,14 +3966,14 @@
       <c r="E15" s="40"/>
       <c r="F15" s="40">
         <f>SUM(D16:D20)</f>
-        <v>25.5</v>
-      </c>
-      <c r="G15" s="150"/>
-      <c r="H15" s="150"/>
+        <v>24</v>
+      </c>
+      <c r="G15" s="127"/>
+      <c r="H15" s="127"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="D16" s="36">
         <v>3</v>
@@ -4803,51 +3981,51 @@
       <c r="E16" s="36">
         <v>3</v>
       </c>
-      <c r="G16" s="150"/>
-      <c r="H16" s="150"/>
+      <c r="G16" s="127"/>
+      <c r="H16" s="127"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="73" t="s">
-        <v>165</v>
+      <c r="A17" s="53" t="s">
+        <v>123</v>
       </c>
       <c r="D17" s="36">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="E17" s="36">
         <v>3</v>
       </c>
-      <c r="G17" s="150"/>
-      <c r="H17" s="150"/>
+      <c r="G17" s="127"/>
+      <c r="H17" s="127"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="73" t="s">
-        <v>166</v>
+      <c r="A18" s="53" t="s">
+        <v>124</v>
       </c>
       <c r="D18" s="36">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="E18" s="36">
         <v>3</v>
       </c>
-      <c r="G18" s="150"/>
-      <c r="H18" s="150"/>
+      <c r="G18" s="127"/>
+      <c r="H18" s="127"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="73" t="s">
-        <v>167</v>
+      <c r="A19" s="53" t="s">
+        <v>125</v>
       </c>
       <c r="D19" s="36">
-        <v>7.5</v>
+        <v>6</v>
       </c>
       <c r="E19" s="36">
         <v>3</v>
       </c>
-      <c r="G19" s="150"/>
-      <c r="H19" s="150"/>
+      <c r="G19" s="127"/>
+      <c r="H19" s="127"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="D20" s="36">
         <v>5</v>
@@ -4855,12 +4033,12 @@
       <c r="E20" s="36">
         <v>3</v>
       </c>
-      <c r="G20" s="150"/>
-      <c r="H20" s="150"/>
+      <c r="G20" s="127"/>
+      <c r="H20" s="127"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="39" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B21" s="40"/>
       <c r="C21" s="40"/>
@@ -4868,14 +4046,14 @@
       <c r="E21" s="40"/>
       <c r="F21" s="40">
         <f>SUM(D22:D26)</f>
-        <v>30</v>
-      </c>
-      <c r="G21" s="150"/>
-      <c r="H21" s="150"/>
+        <v>29</v>
+      </c>
+      <c r="G21" s="127"/>
+      <c r="H21" s="127"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="D22" s="36">
         <v>3</v>
@@ -4887,8 +4065,8 @@
       <c r="H22" s="37"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="73" t="s">
-        <v>165</v>
+      <c r="A23" s="53" t="s">
+        <v>123</v>
       </c>
       <c r="D23" s="36">
         <v>6</v>
@@ -4900,8 +4078,8 @@
       <c r="H23" s="37"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="73" t="s">
-        <v>166</v>
+      <c r="A24" s="53" t="s">
+        <v>124</v>
       </c>
       <c r="D24" s="36">
         <v>8</v>
@@ -4913,11 +4091,11 @@
       <c r="H24" s="37"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="73" t="s">
-        <v>167</v>
+      <c r="A25" s="53" t="s">
+        <v>125</v>
       </c>
       <c r="D25" s="36">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25" s="36">
         <v>3</v>
@@ -4927,7 +4105,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="D26" s="36">
         <v>4</v>
@@ -4940,7 +4118,7 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="39" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B27" s="38"/>
       <c r="C27" s="38"/>
@@ -4955,7 +4133,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="D28" s="36">
         <v>4</v>
@@ -4968,7 +4146,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="D29" s="36">
         <v>8</v>
@@ -4981,7 +4159,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>151</v>
+        <v>109</v>
       </c>
       <c r="D30" s="36">
         <v>2</v>
@@ -4994,7 +4172,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>152</v>
+        <v>110</v>
       </c>
       <c r="D31" s="36">
         <v>4</v>
@@ -5007,7 +4185,7 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="39" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="B32" s="38"/>
       <c r="C32" s="38"/>
@@ -5015,14 +4193,14 @@
       <c r="E32" s="40"/>
       <c r="F32" s="40">
         <f>SUM(D33:D37)</f>
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G32" s="37"/>
       <c r="H32" s="37"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="D33" s="36">
         <v>5</v>
@@ -5035,7 +4213,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
       <c r="D34" s="36">
         <v>4</v>
@@ -5048,7 +4226,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>155</v>
+        <v>113</v>
       </c>
       <c r="D35" s="36">
         <v>9</v>
@@ -5061,10 +4239,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>156</v>
+        <v>114</v>
       </c>
       <c r="D36" s="36">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E36" s="36">
         <v>3</v>
@@ -5074,10 +4252,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="D37" s="36">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E37" s="36">
         <v>3</v>
@@ -5087,297 +4265,110 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="38" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C38" s="38"/>
       <c r="D38" s="38">
         <f>SUM(F3:F32)</f>
-        <v>142.5</v>
+        <v>136</v>
       </c>
       <c r="E38" s="38"/>
       <c r="F38" s="32"/>
       <c r="G38" s="36" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="D40" s="41">
         <f>D38*F40</f>
-        <v>42.75</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="E40" s="33"/>
       <c r="F40" s="46">
         <v>0.3</v>
       </c>
       <c r="G40" s="36" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="34" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C41" s="34"/>
       <c r="D41" s="42">
         <f>SUM(D38:D40)</f>
-        <v>185.25</v>
+        <v>176.8</v>
       </c>
       <c r="E41" s="43"/>
       <c r="F41" s="44"/>
       <c r="G41" s="36" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" s="147" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" s="147"/>
+        <v>59</v>
+      </c>
+      <c r="D44" s="128" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="128"/>
       <c r="F44" s="49">
         <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D45" s="147" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" s="147"/>
+      <c r="D45" s="128" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" s="128"/>
       <c r="F45" s="48">
         <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D46" s="147" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="147"/>
+      <c r="D46" s="128" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" s="128"/>
       <c r="F46" s="48">
         <f>F45*F44</f>
         <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D47" s="147" t="s">
-        <v>80</v>
-      </c>
-      <c r="E47" s="147"/>
+      <c r="D47" s="128" t="s">
+        <v>63</v>
+      </c>
+      <c r="E47" s="128"/>
       <c r="F47" s="47">
         <f>D38/F45</f>
-        <v>15.833333333333334</v>
+        <v>15.111111111111111</v>
       </c>
       <c r="G47" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G8:H21"/>
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:J21"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="98.5703125" style="51" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="51" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="51"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="57" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="152" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="152"/>
-      <c r="F5" s="152"/>
-      <c r="G5" s="152"/>
-      <c r="H5" s="152"/>
-      <c r="I5" s="152"/>
-      <c r="J5" s="152"/>
-    </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="55"/>
-      <c r="D6" s="60">
-        <v>1</v>
-      </c>
-      <c r="E6" s="153" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="154"/>
-      <c r="G6" s="154"/>
-      <c r="H6" s="154"/>
-      <c r="I6" s="154"/>
-      <c r="J6" s="155"/>
-    </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="54" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="55"/>
-      <c r="D7" s="152">
-        <v>2</v>
-      </c>
-      <c r="E7" s="151" t="s">
-        <v>87</v>
-      </c>
-      <c r="F7" s="151"/>
-      <c r="G7" s="151"/>
-      <c r="H7" s="151"/>
-      <c r="I7" s="151"/>
-      <c r="J7" s="151"/>
-    </row>
-    <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="55"/>
-      <c r="D8" s="152"/>
-      <c r="E8" s="151"/>
-      <c r="F8" s="151"/>
-      <c r="G8" s="151"/>
-      <c r="H8" s="151"/>
-      <c r="I8" s="151"/>
-      <c r="J8" s="151"/>
-    </row>
-    <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="55"/>
-      <c r="D9" s="60">
-        <v>3</v>
-      </c>
-      <c r="E9" s="153" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" s="154"/>
-      <c r="G9" s="154"/>
-      <c r="H9" s="154"/>
-      <c r="I9" s="154"/>
-      <c r="J9" s="155"/>
-    </row>
-    <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="55"/>
-    </row>
-    <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" s="55"/>
-    </row>
-    <row r="12" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="54" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="55"/>
-    </row>
-    <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" s="55"/>
-    </row>
-    <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="55"/>
-    </row>
-    <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="55"/>
-    </row>
-    <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" s="55"/>
-    </row>
-    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="54" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="55"/>
-    </row>
-    <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="55"/>
-    </row>
-    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="59">
-        <f>SUM(B6:B18)</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="52" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="52" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="53" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="E7:J8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E6:J6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>